<commit_message>
Results Analysis mostly done
</commit_message>
<xml_diff>
--- a/Darts/Performance Metric - MAE.xlsx
+++ b/Darts/Performance Metric - MAE.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,11 +450,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Floor 3_aggr</t>
+          <t>Floor 10_aggr</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6.950256743968994</v>
+        <v>6.399127039792575</v>
       </c>
     </row>
     <row r="3">
@@ -463,11 +463,102 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Floor 12_aggr</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>6.713001223166926</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Floor 14_aggr</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>7.059946410372695</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Floor 16_aggr</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>8.402791164765512</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Floor 3_aggr</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6.950256743968994</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Floor 4_aggr</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C7" t="n">
         <v>6.772114049023483</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Floor 6_aggr</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7.039346536089296</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Floor 8_aggr</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>6.98998673392105</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>String Pots_aggr</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1.546210047362643</v>
       </c>
     </row>
   </sheetData>
@@ -673,7 +764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -699,11 +790,115 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Floor 10_aggr</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>7.289631405653163</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Floor 12_aggr</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>6.774843235548796</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Floor 14_aggr</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>6.857340676566108</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Floor 16_aggr</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>8.51881499337639</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Floor 3_aggr</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6.984120514459121</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Floor 4_aggr</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6.867393864252254</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Floor 6_aggr</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C8" t="n">
         <v>7.098759493396401</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Floor 8_aggr</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>6.874483117872179</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>String Pots_aggr</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1.184971391881689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>